<commit_message>
add temp vs time
</commit_message>
<xml_diff>
--- a/func/温度.xlsx
+++ b/func/温度.xlsx
@@ -51,6 +51,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="177" formatCode="0.00000000_);[Red]\(0.00000000\)"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -642,7 +645,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -989,17 +992,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2684"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2685" sqref="B2685:J2685"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.25" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B1" t="s">
@@ -86889,5 +86892,6 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>